<commit_message>
* Solved the problem of custom format minute conversion
</commit_message>
<xml_diff>
--- a/easyexcel-test/src/test/resources/dataformat/dataformat.xlsx
+++ b/easyexcel-test/src/test/resources/dataformat/dataformat.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhuangjiaju/IdeaProjects/tmp/easyexcel/src/test/resources/dataformat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lonecloud/Documents/ideaCode/easyexcel/easyexcel-test/src/test/resources/dataformat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E316B3C4-A3FD-084B-81DF-FB975BF9B905}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="55">
   <si>
     <t>date</t>
   </si>
@@ -87,12 +86,6 @@
     <t>1111.11</t>
   </si>
   <si>
-    <t>2020/1/1 1:01 上午</t>
-  </si>
-  <si>
-    <t>2020/1/1 1:01 AM</t>
-  </si>
-  <si>
     <t>1111</t>
   </si>
   <si>
@@ -154,9 +147,6 @@
   </si>
   <si>
     <t>AM1时01分01秒</t>
-  </si>
-  <si>
-    <t>2020年1月1日 1:01:01</t>
   </si>
   <si>
     <t>0.11</t>
@@ -180,14 +170,41 @@
   </si>
   <si>
     <t>5%</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020年1月1日 1:02:01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020年1月1日 1时02分01秒</t>
+  </si>
+  <si>
+    <t>2020/1/1 1:02 上午</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2020/1/1 1:02 AM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1时02分</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>上午1时02分</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>AM1时02分</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="19">
     <numFmt numFmtId="176" formatCode="mmmm/yy"/>
     <numFmt numFmtId="177" formatCode="yy/m/d"/>
     <numFmt numFmtId="178" formatCode="[DBNum1][$-804]yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;"/>
@@ -206,6 +223,7 @@
     <numFmt numFmtId="191" formatCode="m/d"/>
     <numFmt numFmtId="192" formatCode="[DBNum1]h&quot;时&quot;mm&quot;分&quot;"/>
     <numFmt numFmtId="193" formatCode="0.00_ "/>
+    <numFmt numFmtId="194" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;\ h&quot;时&quot;mm&quot;分&quot;ss&quot;秒&quot;"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -298,7 +316,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -424,6 +442,9 @@
     </xf>
     <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -729,17 +750,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="172" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
-    <col min="2" max="3" width="22.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125"/>
     <col min="5" max="5" width="22.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="18" style="1" customWidth="1"/>
@@ -947,22 +969,22 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="19">
-        <v>43831.042372685202</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>43831.043067129627</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>51</v>
       </c>
       <c r="D11" s="20">
         <v>1111.1111000000001</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -970,19 +992,19 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="22">
         <v>1111.1111000000001</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -990,10 +1012,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1010,19 +1032,19 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="40">
         <v>0.105</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17">
@@ -1030,19 +1052,19 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D15" s="41">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1050,10 +1072,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -1061,10 +1083,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1072,10 +1094,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1083,10 +1105,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1094,10 +1116,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1105,10 +1127,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1116,10 +1138,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1127,10 +1149,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1138,10 +1160,10 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1149,47 +1171,55 @@
         <v>43831.042372685202</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="36">
-        <v>43831.042372685202</v>
+        <v>43831.043067129627</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="37">
-        <v>43831.042372685202</v>
+        <v>43831.043067129627</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="38">
-        <v>43831.042372685202</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>44</v>
+        <v>43831.043067129627</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="38"/>
+      <c r="A29" s="42">
+        <v>43831.043067129627</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1199,7 +1229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1213,7 +1243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>